<commit_message>
My 13th commit through Intellij
</commit_message>
<xml_diff>
--- a/src/main/resources/NinzaTestData.xlsx
+++ b/src/main/resources/NinzaTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\IdeaProjects\SeleniumDemo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D98291-4700-4459-82B6-73641C4A0E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12FFC83-9136-4DF5-B660-F27EAB15132E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Campaigns" sheetId="3" r:id="rId1"/>
     <sheet name="Contacts" sheetId="1" r:id="rId2"/>
     <sheet name="Products" sheetId="4" r:id="rId3"/>
+    <sheet name="Login" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Organization</t>
   </si>
@@ -81,16 +82,42 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>http://49.249.28.218:8098/</t>
+  </si>
+  <si>
+    <t>rmgyantra</t>
+  </si>
+  <si>
+    <t>rmgy@9999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,15 +139,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AF93B0-89C6-4514-BC90-A49869839BD3}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -518,4 +564,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43379FB7-7295-4FB8-85DA-F9EDEC0480C4}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E96E243D-E5BD-40CB-840C-57B0E3691F56}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{6349AE08-399A-4117-9088-B6E68D8166E5}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{B7D55D06-3700-487B-ABD8-B224D0289E9B}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{7EA5057A-8B4D-4F7E-83AF-96D8C0C7099A}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{28D04FDB-934F-4750-91E6-B3E36E4DFE12}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{2B906D42-1AAB-4A97-9351-0344CFA77DE1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>